<commit_message>
added sample output file and updated code. Use git pull origin master to get the version to your local repository
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ironzinc/Desktop/Exeter/Lower/Winter/Track/TrackTimer/Timer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B165863D-07E4-1148-88E6-9AA064187A4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE13934E-B306-1541-9C2B-B5C748C5C6DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{BB008B27-5741-9D4E-A959-EB1E9334C01E}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="33">
   <si>
     <t>Name</t>
   </si>
@@ -107,12 +107,6 @@
     <t>The Id of each lap within a run. Resets to 1 in a new run</t>
   </si>
   <si>
-    <t>CumulativeSegmentLength</t>
-  </si>
-  <si>
-    <t>The cumulative length of the run at the end of a segment (one press of the lap button). Determined before a run is made. May or may not be at constant intervals</t>
-  </si>
-  <si>
     <t>The current cumulative time in seconds</t>
   </si>
   <si>
@@ -135,9 +129,6 @@
   </si>
   <si>
     <t>Each time lap button is pressed update a counter, or generate an index column for the lap times numpy array. I can handle this</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This part is tricky. The idea is that we get a list of the values for the cumulative distance at the end of a lap press. We can have coaches enter a list. At the same time we must be aware of the fact that a coach might accidentally press the lap button. Something we can do is to increase robustness is assume that coaches will press the lap button at fixed distances and not make them enter a list before hand (the segment intervals are RunLength/max(SegmentId)) </t>
   </si>
   <si>
     <t>The value outputted by program already</t>
@@ -512,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99321D3A-3CB4-E54A-9222-3F2E08B37CE2}">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -528,12 +519,11 @@
     <col min="6" max="6" width="15.6640625" customWidth="1"/>
     <col min="7" max="7" width="17.33203125" customWidth="1"/>
     <col min="8" max="8" width="20.6640625" customWidth="1"/>
-    <col min="9" max="9" width="34.6640625" customWidth="1"/>
-    <col min="10" max="10" width="16.1640625" customWidth="1"/>
-    <col min="11" max="11" width="44.5" customWidth="1"/>
+    <col min="9" max="9" width="16.1640625" customWidth="1"/>
+    <col min="10" max="10" width="44.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -556,13 +546,10 @@
         <v>5</v>
       </c>
       <c r="I1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -588,13 +575,10 @@
         <v>1</v>
       </c>
       <c r="I2">
-        <v>15</v>
-      </c>
-      <c r="J2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -620,13 +604,10 @@
         <v>2</v>
       </c>
       <c r="I3">
-        <v>30</v>
-      </c>
-      <c r="J3">
         <v>3.2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -652,13 +633,10 @@
         <v>3</v>
       </c>
       <c r="I4">
-        <v>45</v>
-      </c>
-      <c r="J4">
         <v>4.3</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -684,13 +662,10 @@
         <v>4</v>
       </c>
       <c r="I5">
-        <v>60</v>
-      </c>
-      <c r="J5">
         <v>6.1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -716,13 +691,10 @@
         <v>1</v>
       </c>
       <c r="I6">
-        <v>40</v>
-      </c>
-      <c r="J6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -748,13 +720,10 @@
         <v>2</v>
       </c>
       <c r="I7">
-        <v>80</v>
-      </c>
-      <c r="J7">
         <v>10.1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -780,13 +749,10 @@
         <v>3</v>
       </c>
       <c r="I8">
-        <v>120</v>
-      </c>
-      <c r="J8">
         <v>15.2</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -812,13 +778,10 @@
         <v>4</v>
       </c>
       <c r="I9">
-        <v>160</v>
-      </c>
-      <c r="J9">
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -844,13 +807,10 @@
         <v>5</v>
       </c>
       <c r="I10">
-        <v>200</v>
-      </c>
-      <c r="J10">
         <v>25.7</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -876,13 +836,10 @@
         <v>1</v>
       </c>
       <c r="I11">
-        <v>10</v>
-      </c>
-      <c r="J11">
         <v>1.8</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -908,13 +865,10 @@
         <v>2</v>
       </c>
       <c r="I12">
-        <v>30</v>
-      </c>
-      <c r="J12">
         <v>4.7</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -940,13 +894,10 @@
         <v>3</v>
       </c>
       <c r="I13">
-        <v>55</v>
-      </c>
-      <c r="J13">
         <v>7.2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -972,13 +923,10 @@
         <v>1</v>
       </c>
       <c r="I14">
-        <v>400</v>
-      </c>
-      <c r="J14">
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1004,13 +952,10 @@
         <v>2</v>
       </c>
       <c r="I15">
-        <v>800</v>
-      </c>
-      <c r="J15">
         <v>110</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1036,13 +981,10 @@
         <v>3</v>
       </c>
       <c r="I16">
-        <v>1200</v>
-      </c>
-      <c r="J16">
         <v>170.2</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1068,13 +1010,10 @@
         <v>4</v>
       </c>
       <c r="I17">
-        <v>1609</v>
-      </c>
-      <c r="J17">
         <v>250.3</v>
       </c>
     </row>
-    <row r="22" spans="1:11" s="1" customFormat="1" ht="182" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" s="1" customFormat="1" ht="182" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>18</v>
       </c>
@@ -1100,48 +1039,42 @@
         <v>23</v>
       </c>
       <c r="I22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J22" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J22" s="1" t="s">
+    </row>
+    <row r="25" spans="1:10" ht="220" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J25" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="K22" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="220" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="K25" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>